<commit_message>
implemented RTL source file generation
</commit_message>
<xml_diff>
--- a/sample/block_0.xlsx
+++ b/sample/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B053033C-F627-4304-B8B9-A7A7A71CD5E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B687BEE-852B-4EC1-8B9A-A9549027B4FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -106,33 +106,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ro</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bit_field_4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>24:4</t>
-  </si>
-  <si>
-    <t>register_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x04</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>8:4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>16:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>rc</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -145,10 +126,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>0x08</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -201,10 +178,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>w1s</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -233,15 +206,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0x30</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>[2, 4]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -261,6 +226,66 @@
 register_0.bit_field_0
 register_0.bit_field_1
 register_0.bit_field_2:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x04</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ro</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x20</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x40</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>20:4</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -867,7 +892,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J25"/>
+  <dimension ref="B1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -973,10 +998,10 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
@@ -992,18 +1017,22 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
@@ -1014,34 +1043,34 @@
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="26" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="28"/>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
@@ -1054,63 +1083,61 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -1119,27 +1146,25 @@
       <c r="D14" s="24"/>
       <c r="E14" s="25"/>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="28"/>
@@ -1147,50 +1172,56 @@
         <v>12</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
+      <c r="B17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
@@ -1203,19 +1234,19 @@
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I18" s="4">
         <v>0</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1224,57 +1255,53 @@
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
       <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="H21" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -1287,37 +1314,35 @@
       <c r="D22" s="24"/>
       <c r="E22" s="25"/>
       <c r="F22" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10" ht="75">
+    <row r="23" spans="2:10">
       <c r="B23" s="26" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>59</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E23" s="28"/>
       <c r="F23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>14</v>
@@ -1336,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>14</v>
@@ -1346,24 +1371,70 @@
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="9"/>
+    <row r="25" spans="2:10" ht="75">
+      <c r="B25" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
updated setup file and samples
</commit_message>
<xml_diff>
--- a/sample/block_0.xlsx
+++ b/sample/block_0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B90691D-6333-4AD0-B06B-D31C74B91901}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0ADD80-03F7-4649-8CE9-036AF7D62EF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -314,6 +314,46 @@
   </si>
   <si>
     <t>register_5.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ro</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rof</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xab</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reserved</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -920,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J30"/>
+  <dimension ref="B1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1066,81 +1106,75 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="3" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="3" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="I11" s="4"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="26" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="28"/>
       <c r="F12" s="3" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
@@ -1153,82 +1187,80 @@
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="3" t="s">
+    <row r="16" spans="2:10">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -1237,27 +1269,25 @@
       <c r="D17" s="24"/>
       <c r="E17" s="25"/>
       <c r="F17" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="28"/>
@@ -1265,55 +1295,61 @@
         <v>12</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I18" s="4">
         <v>0</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="20"/>
@@ -1321,18 +1357,20 @@
       <c r="D21" s="21"/>
       <c r="E21" s="22"/>
       <c r="F21" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="20"/>
@@ -1340,19 +1378,17 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="5" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -1361,18 +1397,18 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5" t="s">
-        <v>72</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="20"/>
@@ -1380,57 +1416,53 @@
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
       <c r="F24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1443,32 +1475,30 @@
       <c r="D27" s="24"/>
       <c r="E27" s="25"/>
       <c r="F27" s="3" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10" ht="75">
+    <row r="28" spans="2:10">
       <c r="B28" s="26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>50</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E28" s="28"/>
       <c r="F28" s="3" t="s">
         <v>12</v>
       </c>
@@ -1502,24 +1532,70 @@
       </c>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="2:10" ht="75">
+      <c r="B30" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="9"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
updated samples to add w0trg and w1trg bit field types
</commit_message>
<xml_diff>
--- a/sample/block_0.xlsx
+++ b/sample/block_0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495EF139-AD97-4388-9E44-FBB4578E4D3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8194F90-CF7D-4B7C-B011-DE5ED76A6BC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -237,6 +237,66 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>register_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x20</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x40</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>20:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>28:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_5.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_5.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>bit_field_1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -245,63 +305,39 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x20</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x40</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>28:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_5.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_5.bit_field_4</t>
+    <t>ro</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rof</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xab</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rwc</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -309,27 +345,26 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>4:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rwc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>8:4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ro</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rof</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0xab</t>
+    <t>rwe</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -337,15 +372,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>24:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwc</t>
+    <t>12:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rwl</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -353,50 +392,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>4:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>12:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwl</t>
+    <t>8:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_2.bit_field_1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1003,7 +1015,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J36"/>
+  <dimension ref="B1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1154,13 +1166,13 @@
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
       <c r="F9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
@@ -1171,16 +1183,16 @@
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1190,20 +1202,20 @@
       <c r="D11" s="24"/>
       <c r="E11" s="25"/>
       <c r="F11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>49</v>
@@ -1217,7 +1229,7 @@
         <v>51</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
@@ -1230,52 +1242,48 @@
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="3" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="3" t="s">
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>23</v>
@@ -1283,9 +1291,7 @@
       <c r="I15" s="4">
         <v>0</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="20"/>
@@ -1293,81 +1299,81 @@
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="3" t="s">
+      <c r="I17" s="4"/>
+      <c r="J17" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="26" t="s">
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="3" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="20"/>
@@ -1375,18 +1381,20 @@
       <c r="D20" s="21"/>
       <c r="E20" s="22"/>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="20"/>
@@ -1394,20 +1402,18 @@
       <c r="D21" s="21"/>
       <c r="E21" s="22"/>
       <c r="F21" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="20"/>
@@ -1415,73 +1421,75 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="G24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="26" t="s">
+    <row r="25" spans="2:10">
+      <c r="B25" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C25" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="3" t="s">
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>31</v>
@@ -1489,9 +1497,7 @@
       <c r="I25" s="4">
         <v>0</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="20"/>
@@ -1499,17 +1505,19 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
       <c r="J26" s="5" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -1518,18 +1526,18 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="20"/>
@@ -1537,10 +1545,10 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>32</v>
@@ -1548,9 +1556,7 @@
       <c r="I28" s="4">
         <v>0</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="20"/>
@@ -1558,17 +1564,19 @@
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
       <c r="J29" s="5" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:10">
@@ -1577,73 +1585,73 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="4">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="3" t="s">
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I31" s="4">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="27" t="s">
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="3" t="s">
+      <c r="E33" s="28"/>
+      <c r="F33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="4">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>14</v>
@@ -1653,24 +1661,16 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="2:10" ht="75">
-      <c r="B34" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>47</v>
-      </c>
+    <row r="34" spans="2:10">
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
       <c r="F34" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>14</v>
@@ -1680,16 +1680,24 @@
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
+    <row r="35" spans="2:10" ht="75">
+      <c r="B35" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>47</v>
+      </c>
       <c r="F35" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>14</v>
@@ -1699,24 +1707,43 @@
       </c>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="2:10">
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="9"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>